<commit_message>
Updated with project 1)sort and filter and then upload oto Web
</commit_message>
<xml_diff>
--- a/Project_google_search_method.xlsx
+++ b/Project_google_search_method.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shubham\Desktop\RPA\MyProjects\Calculator Demo\My First Process\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A861755A-AC29-4345-8AD8-FF4A97B7A286}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCC25D79-D90C-42E7-BFD0-ACFAB118FC05}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4005" yWindow="2820" windowWidth="15375" windowHeight="7965" xr2:uid="{3FF96EE3-CE1E-4C10-8AAD-DFA50C7CF3AC}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11280" xr2:uid="{3FF96EE3-CE1E-4C10-8AAD-DFA50C7CF3AC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -39,83 +39,91 @@
     <t>URL</t>
   </si>
   <si>
-    <t>Top 5 Best-Paying Networking Jobs | Network Computing</t>
-  </si>
-  <si>
-    <t>https://www.networkcomputing.com/networking/top-5-best-paying-networking-jobs</t>
-  </si>
-  <si>
-    <t>https://www.cybrary.it/blog/2018/06/network-engineering-good-career/</t>
-  </si>
-  <si>
-    <t>https://www.foxbusiness.com/lifestyle/the-10-highest-paying-jobs-in-the-world</t>
-  </si>
-  <si>
-    <t>https://www.businessnewsdaily.com/10776-networking-career.html</t>
-  </si>
-  <si>
-    <t>https://www.computerweekly.com/feature/Networking-or-programming-which-has-the-better-prospects</t>
-  </si>
-  <si>
-    <t>Top 5 Highest Paying Jobs in Networking - GeeksforGeeks</t>
-  </si>
-  <si>
-    <t>https://www.geeksforgeeks.org/top-5-highest-paying-jobs-in-networking/</t>
-  </si>
-  <si>
-    <t>5 Highest Paying Networking Jobs - NetCom Learning</t>
-  </si>
-  <si>
-    <t>https://www.netcomlearning.com/blogs/80/144/5-Highest-Paying-Networking-Jobs.html</t>
-  </si>
-  <si>
-    <t>10 best IT jobs right now | Network World</t>
-  </si>
-  <si>
-    <t>https://www.networkworld.com/article/2243453/10-best-it-jobs-right-now.html</t>
-  </si>
-  <si>
-    <t>Advance Your Networking Career - Business News Daily</t>
-  </si>
-  <si>
-    <t>Networking Jobs (Sep 2020) - Latest Networking Job ...</t>
-  </si>
-  <si>
-    <t>https://www.monsterindia.com/search/networking-jobs</t>
-  </si>
-  <si>
-    <t>Best Computer Jobs for the Future | Top 10 IT Careers 2020 ...</t>
-  </si>
-  <si>
-    <t>https://www.itcareerfinder.com/brain-food/blog/entry/best-computer-jobs-for-the-future.html</t>
-  </si>
-  <si>
-    <t>Network Engineer Jobs In Abroad - 60 Network Engineer ...</t>
-  </si>
-  <si>
-    <t>https://www.naukri.com/network-engineer-jobs-in-abroad</t>
-  </si>
-  <si>
-    <t>13 Highest-Paying IT Jobs | Robert Half</t>
-  </si>
-  <si>
-    <t>https://www.roberthalf.com/blog/salaries-and-skills/the-13-highest-paying-it-jobs-in-2019</t>
-  </si>
-  <si>
-    <t>Top companies in world for network engineer jobs</t>
-  </si>
-  <si>
-    <t>https://www.cos.youth4work.com/jobs/work-in-world-for-network-engineer/4</t>
+    <t>Europe's Most Livable Cities | Far &amp; Wide</t>
+  </si>
+  <si>
+    <t>https://www.farandwide.com/s/europes-most-livable-cities-71985994306c4df6</t>
+  </si>
+  <si>
+    <t>https://ilovemoving.com/best-european-country-to-live-in/</t>
+  </si>
+  <si>
+    <t>http://www.linksmoving.asia/blog/cheapest-european-countries-for-expats/</t>
+  </si>
+  <si>
+    <t>https://www.cntraveler.com/gallery/countries-with-best-work-life-balance-in-europe</t>
+  </si>
+  <si>
+    <t>https://www.glassdoor.com/research/app/uploads/sites/2/2016/04/Wages_StandardofLiving_Final-2.pdf</t>
+  </si>
+  <si>
+    <t>Best destinations to live in Europe if you want to leave the USA</t>
+  </si>
+  <si>
+    <t>https://www.europeanbestdestinations.com/best-of-europe/best-destinations-to-live-in-europe-if-you-want-to-leave-the-usa/</t>
+  </si>
+  <si>
+    <t>Best Places to Live in Europe - Nomad List</t>
+  </si>
+  <si>
+    <t>https://nomadlist.com/europe</t>
+  </si>
+  <si>
+    <t>The 24 European cities with the best quality of life - Business ...</t>
+  </si>
+  <si>
+    <t>https://www.businessinsider.com/the-24-european-cities-with-the-best-quality-of-life-2018-8</t>
+  </si>
+  <si>
+    <t>Top 7 Cities in Europe to Find Work Right Now | MoveHub</t>
+  </si>
+  <si>
+    <t>https://www.movehub.com/blog/top-7-cities-europe-work-now/</t>
+  </si>
+  <si>
+    <t>The 5 Cheapest European Cities to Relocate To in 2020</t>
+  </si>
+  <si>
+    <t>https://www.europelanguagejobs.com/blog/5-cheapest-european-cities-to-relocate-to-in-2020</t>
+  </si>
+  <si>
+    <t>How to Find the Best European Country To Live In - I Love ...</t>
+  </si>
+  <si>
+    <t>Best Places for American Expats to Live Abroad in Europe ...</t>
+  </si>
+  <si>
+    <t>https://shehitrefresh.com/best-places-to-live-in-europe/</t>
+  </si>
+  <si>
+    <t>Best Places to Live in Europe for Digital Nomads in 2020</t>
+  </si>
+  <si>
+    <t>https://wifitribe.co/blog/best-places-to-live-in-europe/</t>
+  </si>
+  <si>
+    <t>10 Cheapest Countries To Live In Europe In 2020 For Expats</t>
+  </si>
+  <si>
+    <t>https://www.budgettravelbuff.com/cheapest-countries-to-live-in-europe/</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -138,13 +146,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -459,9 +470,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4E0A51E-CD92-4B7B-9B19-7A9C15F0ABA4}">
   <dimension ref="A1:B15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="58.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="89.42578125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -475,7 +492,7 @@
       <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
     </row>
@@ -485,7 +502,7 @@
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
+      <c r="B4" s="1" t="s">
         <v>5</v>
       </c>
     </row>
@@ -527,24 +544,24 @@
       <c r="A10" t="s">
         <v>14</v>
       </c>
-      <c r="B10" t="s">
-        <v>6</v>
+      <c r="B10" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B11" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B12" t="s">
-        <v>18</v>
+        <v>4</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -572,6 +589,11 @@
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B10" r:id="rId1" display="https://www.holidify.com/collections/solo-travel-india" xr:uid="{29644813-57FF-4B7C-A2B2-65E9D39BB343}"/>
+    <hyperlink ref="B4" r:id="rId2" display="https://www.travelandleisure.com/trip-ideas/solo-travel/best-countries-for-solo-travelers" xr:uid="{51A423DC-CFE9-4D71-B716-C65161B259E7}"/>
+    <hyperlink ref="B2" r:id="rId3" xr:uid="{81792EFA-8702-4F30-94EC-F3EE139B70F0}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>